<commit_message>
Rerun of terminology v. 1.0.0
Done to handle errors in FHIR registry
</commit_message>
<xml_diff>
--- a/ig/terminology/1.0.0/CodeSystem-medcom-acknowledgement-issue-details.xlsx
+++ b/ig/terminology/1.0.0/CodeSystem-medcom-acknowledgement-issue-details.xlsx
@@ -266,10 +266,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true" applyFont="true">
       <alignment vertical="top" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment vertical="top" wrapText="true"/>
     </xf>
   </cellXfs>

</xml_diff>